<commit_message>
Uopdate RDS IP address patterns to reflect subnet address space
</commit_message>
<xml_diff>
--- a/new_dsg_environment/azure-runbooks/DSG Environment Configuration Checklist.xlsx
+++ b/new_dsg_environment/azure-runbooks/DSG Environment Configuration Checklist.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/moreilly/Source/Turing/data-safe-haven/new_dsg_environment/azure-runbooks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{28A8B473-9ABD-284C-BC81-160FD08D011C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F33A6FA-F6CA-B643-8B66-7393880B54F1}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="600" windowWidth="29320" windowHeight="19320" xr2:uid="{F8504295-A934-4B8B-B17E-A3BEC205C8B4}"/>
+    <workbookView xWindow="12800" yWindow="4360" windowWidth="29320" windowHeight="19320" xr2:uid="{F8504295-A934-4B8B-B17E-A3BEC205C8B4}"/>
   </bookViews>
   <sheets>
     <sheet name="IP Addressing" sheetId="1" r:id="rId1"/>
@@ -26,6 +26,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -82,7 +83,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="119">
   <si>
     <t>DSG Name</t>
   </si>
@@ -414,6 +415,500 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
+      <t>.151</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>10.250.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>x</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.152</t>
+    </r>
+  </si>
+  <si>
+    <t>DSG8</t>
+  </si>
+  <si>
+    <t>DSG9</t>
+  </si>
+  <si>
+    <t>DSG10</t>
+  </si>
+  <si>
+    <t>10.250.56.0/21</t>
+  </si>
+  <si>
+    <t>10.250.64.0/21</t>
+  </si>
+  <si>
+    <t>10.250.72.0/21</t>
+  </si>
+  <si>
+    <t>Service Accounts:</t>
+  </si>
+  <si>
+    <t>User Description</t>
+  </si>
+  <si>
+    <t>User Name</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <r>
+      <t>DSG</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>x</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Data Science LDAP User</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>DSG</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>x</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> GitLab LDAP User</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>DSG</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>x</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> HackMD LDAP User</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>DSG</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>x</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Test User</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>dsg</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>X</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>dsguldap</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>dsg</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>X</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>gitlabldap</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>dsg</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>X</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>hackmdldap</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>dsg</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>X</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>testuser</t>
+    </r>
+  </si>
+  <si>
+    <t>VM/Domain Admin</t>
+  </si>
+  <si>
+    <t>GitLab root</t>
+  </si>
+  <si>
+    <t>DSG Environment</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>RADIUS Secret (Global NPS Server)</t>
+  </si>
+  <si>
+    <t>Services:</t>
+  </si>
+  <si>
+    <t>Management Environment</t>
+  </si>
+  <si>
+    <t>Domain Service Accounts:</t>
+  </si>
+  <si>
+    <t>n/a</t>
+  </si>
+  <si>
+    <t>VPN P2S SSL Certificate</t>
+  </si>
+  <si>
+    <t>root</t>
+  </si>
+  <si>
+    <t>Storage Account</t>
+  </si>
+  <si>
+    <t>Data Study Group Environment Configuration - Network</t>
+  </si>
+  <si>
+    <t>Data Study Group Environment Configuration - Service/User Accounts</t>
+  </si>
+  <si>
+    <t>Blob</t>
+  </si>
+  <si>
+    <t>URL</t>
+  </si>
+  <si>
+    <t>SAS Token</t>
+  </si>
+  <si>
+    <t>File Share</t>
+  </si>
+  <si>
+    <t>PowerShell Connection String</t>
+  </si>
+  <si>
+    <t>Data Study Group Environment Configuration - Azure</t>
+  </si>
+  <si>
+    <t>Resource Group</t>
+  </si>
+  <si>
+    <t>Virtual Network</t>
+  </si>
+  <si>
+    <t>File Share Name</t>
+  </si>
+  <si>
+    <t>RG_DSG_DC</t>
+  </si>
+  <si>
+    <t>RG_DSG_DATASERVER</t>
+  </si>
+  <si>
+    <t>RG_DSG_RDS</t>
+  </si>
+  <si>
+    <t>RG_DSG_LINUX</t>
+  </si>
+  <si>
+    <t>Data Study Group Environment Configuration - Management Environment</t>
+  </si>
+  <si>
+    <t>Domain Name</t>
+  </si>
+  <si>
+    <t>Domain Controller Name</t>
+  </si>
+  <si>
+    <t>Domain Controller IP Address</t>
+  </si>
+  <si>
+    <t>Network Policy Server Name</t>
+  </si>
+  <si>
+    <t>Network Policy Server IP Address</t>
+  </si>
+  <si>
+    <t>Domain Admin Account</t>
+  </si>
+  <si>
+    <t>FQDN of Management Domain</t>
+  </si>
+  <si>
+    <t>OU Path to HackMD LDAP User</t>
+  </si>
+  <si>
+    <t>OU Path to GitLab LDAP User</t>
+  </si>
+  <si>
+    <t>Path to Safe Haven Reseach Users OU</t>
+  </si>
+  <si>
+    <r>
+      <t>10.250.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>x+1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.0/24</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>10.250.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>x+2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.0/24</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>10.250.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>x+7</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.0/27</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>10.250.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>x+1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.250</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>10.250.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>x+1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>.249</t>
     </r>
   </si>
@@ -429,7 +924,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>x</t>
+      <t>x+1</t>
     </r>
     <r>
       <rPr>
@@ -440,475 +935,6 @@
         <scheme val="minor"/>
       </rPr>
       <t>.248</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>10.250.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>x</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.151</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>10.250.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>x</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.152</t>
-    </r>
-  </si>
-  <si>
-    <t>DSG8</t>
-  </si>
-  <si>
-    <t>DSG9</t>
-  </si>
-  <si>
-    <t>DSG10</t>
-  </si>
-  <si>
-    <t>10.250.56.0/21</t>
-  </si>
-  <si>
-    <t>10.250.64.0/21</t>
-  </si>
-  <si>
-    <t>10.250.72.0/21</t>
-  </si>
-  <si>
-    <t>Service Accounts:</t>
-  </si>
-  <si>
-    <t>User Description</t>
-  </si>
-  <si>
-    <t>User Name</t>
-  </si>
-  <si>
-    <t>Password</t>
-  </si>
-  <si>
-    <r>
-      <t>DSG</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>x</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Data Science LDAP User</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>DSG</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>x</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> GitLab LDAP User</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>DSG</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>x</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> HackMD LDAP User</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>DSG</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>x</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Test User</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>dsg</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>X</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>dsguldap</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>dsg</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>X</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>gitlabldap</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>dsg</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>X</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>hackmdldap</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>dsg</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>X</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>testuser</t>
-    </r>
-  </si>
-  <si>
-    <t>VM/Domain Admin</t>
-  </si>
-  <si>
-    <t>GitLab root</t>
-  </si>
-  <si>
-    <t>DSG Environment</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t>RADIUS Secret (Global NPS Server)</t>
-  </si>
-  <si>
-    <t>Services:</t>
-  </si>
-  <si>
-    <t>Management Environment</t>
-  </si>
-  <si>
-    <t>Domain Service Accounts:</t>
-  </si>
-  <si>
-    <t>n/a</t>
-  </si>
-  <si>
-    <t>VPN P2S SSL Certificate</t>
-  </si>
-  <si>
-    <t>root</t>
-  </si>
-  <si>
-    <t>Storage Account</t>
-  </si>
-  <si>
-    <t>Data Study Group Environment Configuration - Network</t>
-  </si>
-  <si>
-    <t>Data Study Group Environment Configuration - Service/User Accounts</t>
-  </si>
-  <si>
-    <t>Blob</t>
-  </si>
-  <si>
-    <t>URL</t>
-  </si>
-  <si>
-    <t>SAS Token</t>
-  </si>
-  <si>
-    <t>File Share</t>
-  </si>
-  <si>
-    <t>PowerShell Connection String</t>
-  </si>
-  <si>
-    <t>Data Study Group Environment Configuration - Azure</t>
-  </si>
-  <si>
-    <t>Resource Group</t>
-  </si>
-  <si>
-    <t>Virtual Network</t>
-  </si>
-  <si>
-    <t>File Share Name</t>
-  </si>
-  <si>
-    <t>RG_DSG_DC</t>
-  </si>
-  <si>
-    <t>RG_DSG_DATASERVER</t>
-  </si>
-  <si>
-    <t>RG_DSG_RDS</t>
-  </si>
-  <si>
-    <t>RG_DSG_LINUX</t>
-  </si>
-  <si>
-    <t>Data Study Group Environment Configuration - Management Environment</t>
-  </si>
-  <si>
-    <t>Domain Name</t>
-  </si>
-  <si>
-    <t>Domain Controller Name</t>
-  </si>
-  <si>
-    <t>Domain Controller IP Address</t>
-  </si>
-  <si>
-    <t>Network Policy Server Name</t>
-  </si>
-  <si>
-    <t>Network Policy Server IP Address</t>
-  </si>
-  <si>
-    <t>Domain Admin Account</t>
-  </si>
-  <si>
-    <t>FQDN of Management Domain</t>
-  </si>
-  <si>
-    <t>OU Path to HackMD LDAP User</t>
-  </si>
-  <si>
-    <t>OU Path to GitLab LDAP User</t>
-  </si>
-  <si>
-    <t>Path to Safe Haven Reseach Users OU</t>
-  </si>
-  <si>
-    <r>
-      <t>10.250.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>x+1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.0/24</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>10.250.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>x+2</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.0/24</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>10.250.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>x+7</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.0/27</t>
     </r>
   </si>
 </sst>
@@ -1418,7 +1444,7 @@
   <dimension ref="B2:L30"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1437,7 +1463,7 @@
   <sheetData>
     <row r="2" spans="2:12" ht="19" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2"/>
@@ -1449,7 +1475,7 @@
     </row>
     <row r="4" spans="2:12" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C4" s="3"/>
     </row>
@@ -1469,7 +1495,7 @@
         <v>13</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>1</v>
@@ -1510,13 +1536,13 @@
         <v>51</v>
       </c>
       <c r="G7" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="I7" s="6" t="s">
         <v>115</v>
-      </c>
-      <c r="H7" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="I7" s="6" t="s">
-        <v>117</v>
       </c>
       <c r="K7" s="6" t="s">
         <v>37</v>
@@ -1568,7 +1594,7 @@
         <v>8</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E11" s="5" t="s">
         <v>9</v>
@@ -1600,7 +1626,7 @@
         <v>14</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E12" s="6" t="s">
         <v>54</v>
@@ -1619,18 +1645,18 @@
         <v>15</v>
       </c>
       <c r="K12" s="6" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="L12" s="6" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13" spans="2:12" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K13" s="6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="L13" s="6" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="14" spans="2:12" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1638,10 +1664,10 @@
         <v>17</v>
       </c>
       <c r="K14" s="6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="L14" s="6" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="15" spans="2:12" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1653,7 +1679,7 @@
         <v>8</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E16" s="5" t="s">
         <v>9</v>
@@ -1679,7 +1705,7 @@
         <v>14</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E17" s="6" t="s">
         <v>53</v>
@@ -1717,7 +1743,7 @@
         <v>8</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="F21" s="5" t="s">
         <v>9</v>
@@ -1746,10 +1772,10 @@
         <v>20</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F22" s="6" t="s">
-        <v>54</v>
+        <v>116</v>
       </c>
       <c r="G22" s="6" t="s">
         <v>3</v>
@@ -1781,7 +1807,7 @@
         <v>RG_DSG_RDS</v>
       </c>
       <c r="F23" s="6" t="s">
-        <v>55</v>
+        <v>117</v>
       </c>
       <c r="G23" s="6" t="s">
         <v>3</v>
@@ -1813,7 +1839,7 @@
         <v>RG_DSG_RDS</v>
       </c>
       <c r="F24" s="6" t="s">
-        <v>56</v>
+        <v>118</v>
       </c>
       <c r="G24" s="6" t="s">
         <v>3</v>
@@ -1848,7 +1874,7 @@
         <v>8</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="F28" s="5" t="s">
         <v>9</v>
@@ -1877,10 +1903,10 @@
         <v>14</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F29" s="6" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="G29" s="6" t="s">
         <v>4</v>
@@ -1912,7 +1938,7 @@
         <v>RG_DSG_LINUX</v>
       </c>
       <c r="F30" s="6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="G30" s="6" t="s">
         <v>4</v>
@@ -1954,7 +1980,7 @@
   <sheetData>
     <row r="2" spans="2:4" ht="19" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" spans="2:4" ht="19" x14ac:dyDescent="0.25">
@@ -1962,90 +1988,90 @@
     </row>
     <row r="4" spans="2:4" ht="19" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B6" s="8" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B8" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="D8" s="10" t="s">
         <v>66</v>
-      </c>
-      <c r="C8" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="D8" s="10" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B9" s="9" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D9" s="9"/>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B10" s="9" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D10" s="9"/>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B11" s="9" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D11" s="9"/>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B12" s="9" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D12" s="9"/>
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B14" s="8" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B16" s="10" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D16" s="10" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B17" s="9" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D17" s="9"/>
     </row>
     <row r="18" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="19" spans="2:5" ht="19" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="20" spans="2:5" ht="19" x14ac:dyDescent="0.25">
@@ -2053,23 +2079,23 @@
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B21" s="8" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B23" s="10" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D23" s="10" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B24" s="9" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C24" s="9" t="s">
         <v>15</v>
@@ -2078,36 +2104,36 @@
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B25" s="13" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D25" s="9"/>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B27" s="8" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B29" s="10" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C29" s="10" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D29" s="24" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E29" s="25"/>
     </row>
     <row r="30" spans="2:5" ht="276" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B30" s="11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C30" s="11" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D30" s="22"/>
       <c r="E30" s="23"/>
@@ -2139,37 +2165,37 @@
     <row r="1" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="3" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="4" spans="2:3" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="5" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C4" s="11"/>
     </row>
     <row r="5" spans="2:3" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="5" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C5" s="11"/>
     </row>
     <row r="6" spans="2:3" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="5" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C6" s="11"/>
     </row>
     <row r="7" spans="2:3" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="5" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C7" s="11"/>
     </row>
     <row r="8" spans="2:3" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="20" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C8" s="21"/>
     </row>
@@ -2179,32 +2205,32 @@
     </row>
     <row r="10" spans="2:3" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="5" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C10" s="11"/>
     </row>
     <row r="11" spans="2:3" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="5" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C11" s="11"/>
     </row>
     <row r="12" spans="2:3" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="13" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B13" s="5" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C13" s="9"/>
     </row>
     <row r="14" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B14" s="5" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C14" s="9"/>
     </row>
     <row r="15" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B15" s="5" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C15" s="9"/>
     </row>
@@ -2229,7 +2255,7 @@
   <sheetData>
     <row r="2" spans="2:5" ht="19" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="3" spans="2:5" ht="19" x14ac:dyDescent="0.25">
@@ -2237,20 +2263,20 @@
     </row>
     <row r="4" spans="2:5" ht="19" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B6" s="14" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B8" s="15" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C8" s="15" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="9" spans="2:5" ht="70.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2259,7 +2285,7 @@
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B11" s="14" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.2">
@@ -2269,10 +2295,10 @@
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B13" s="17" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C13" s="17" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D13" s="16"/>
       <c r="E13" s="16"/>
@@ -2295,6 +2321,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101009C7E73EE9996324088E1F0A060CA721D" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="dd7030be88c7340c0a587c8a356762f5">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="25f20417-b9ad-4008-9f3b-001566dfe55b" xmlns:ns3="1d2e2500-3e90-4d86-b07a-7c1ab3045675" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d01a9fba4890ed2f5624257697a5e155" ns2:_="" ns3:_="">
     <xsd:import namespace="25f20417-b9ad-4008-9f3b-001566dfe55b"/>
@@ -2497,22 +2538,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E5A8AB7A-03D3-43F4-9031-51907E0F9EE1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="1d2e2500-3e90-4d86-b07a-7c1ab3045675"/>
+    <ds:schemaRef ds:uri="25f20417-b9ad-4008-9f3b-001566dfe55b"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AA99EF82-7495-4E7E-A356-9C8544A35D59}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8EB34A6E-743B-4B0F-9C63-84E598C6053C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2529,29 +2580,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AA99EF82-7495-4E7E-A356-9C8544A35D59}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E5A8AB7A-03D3-43F4-9031-51907E0F9EE1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="1d2e2500-3e90-4d86-b07a-7c1ab3045675"/>
-    <ds:schemaRef ds:uri="25f20417-b9ad-4008-9f3b-001566dfe55b"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Update subnet prefix for Data subnet for Data, Gitlab and HackMD servers
</commit_message>
<xml_diff>
--- a/new_dsg_environment/azure-runbooks/DSG Environment Configuration Checklist.xlsx
+++ b/new_dsg_environment/azure-runbooks/DSG Environment Configuration Checklist.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/moreilly/Source/Turing/data-safe-haven/new_dsg_environment/azure-runbooks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F33A6FA-F6CA-B643-8B66-7393880B54F1}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93F0DFA0-4884-8242-AC09-35E038F54CB1}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12800" yWindow="4360" windowWidth="29320" windowHeight="19320" xr2:uid="{F8504295-A934-4B8B-B17E-A3BEC205C8B4}"/>
+    <workbookView xWindow="9080" yWindow="4360" windowWidth="29320" windowHeight="19320" xr2:uid="{F8504295-A934-4B8B-B17E-A3BEC205C8B4}"/>
   </bookViews>
   <sheets>
     <sheet name="IP Addressing" sheetId="1" r:id="rId1"/>
@@ -365,576 +365,576 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
+      <t>.250</t>
+    </r>
+  </si>
+  <si>
+    <t>DSG8</t>
+  </si>
+  <si>
+    <t>DSG9</t>
+  </si>
+  <si>
+    <t>DSG10</t>
+  </si>
+  <si>
+    <t>10.250.56.0/21</t>
+  </si>
+  <si>
+    <t>10.250.64.0/21</t>
+  </si>
+  <si>
+    <t>10.250.72.0/21</t>
+  </si>
+  <si>
+    <t>Service Accounts:</t>
+  </si>
+  <si>
+    <t>User Description</t>
+  </si>
+  <si>
+    <t>User Name</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <r>
+      <t>DSG</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>x</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Data Science LDAP User</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>DSG</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>x</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> GitLab LDAP User</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>DSG</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>x</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> HackMD LDAP User</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>DSG</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>x</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Test User</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>dsg</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>X</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>dsguldap</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>dsg</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>X</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>gitlabldap</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>dsg</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>X</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>hackmdldap</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>dsg</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>X</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>testuser</t>
+    </r>
+  </si>
+  <si>
+    <t>VM/Domain Admin</t>
+  </si>
+  <si>
+    <t>GitLab root</t>
+  </si>
+  <si>
+    <t>DSG Environment</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>RADIUS Secret (Global NPS Server)</t>
+  </si>
+  <si>
+    <t>Services:</t>
+  </si>
+  <si>
+    <t>Management Environment</t>
+  </si>
+  <si>
+    <t>Domain Service Accounts:</t>
+  </si>
+  <si>
+    <t>n/a</t>
+  </si>
+  <si>
+    <t>VPN P2S SSL Certificate</t>
+  </si>
+  <si>
+    <t>root</t>
+  </si>
+  <si>
+    <t>Storage Account</t>
+  </si>
+  <si>
+    <t>Data Study Group Environment Configuration - Network</t>
+  </si>
+  <si>
+    <t>Data Study Group Environment Configuration - Service/User Accounts</t>
+  </si>
+  <si>
+    <t>Blob</t>
+  </si>
+  <si>
+    <t>URL</t>
+  </si>
+  <si>
+    <t>SAS Token</t>
+  </si>
+  <si>
+    <t>File Share</t>
+  </si>
+  <si>
+    <t>PowerShell Connection String</t>
+  </si>
+  <si>
+    <t>Data Study Group Environment Configuration - Azure</t>
+  </si>
+  <si>
+    <t>Resource Group</t>
+  </si>
+  <si>
+    <t>Virtual Network</t>
+  </si>
+  <si>
+    <t>File Share Name</t>
+  </si>
+  <si>
+    <t>RG_DSG_DC</t>
+  </si>
+  <si>
+    <t>RG_DSG_DATASERVER</t>
+  </si>
+  <si>
+    <t>RG_DSG_RDS</t>
+  </si>
+  <si>
+    <t>RG_DSG_LINUX</t>
+  </si>
+  <si>
+    <t>Data Study Group Environment Configuration - Management Environment</t>
+  </si>
+  <si>
+    <t>Domain Name</t>
+  </si>
+  <si>
+    <t>Domain Controller Name</t>
+  </si>
+  <si>
+    <t>Domain Controller IP Address</t>
+  </si>
+  <si>
+    <t>Network Policy Server Name</t>
+  </si>
+  <si>
+    <t>Network Policy Server IP Address</t>
+  </si>
+  <si>
+    <t>Domain Admin Account</t>
+  </si>
+  <si>
+    <t>FQDN of Management Domain</t>
+  </si>
+  <si>
+    <t>OU Path to HackMD LDAP User</t>
+  </si>
+  <si>
+    <t>OU Path to GitLab LDAP User</t>
+  </si>
+  <si>
+    <t>Path to Safe Haven Reseach Users OU</t>
+  </si>
+  <si>
+    <r>
+      <t>10.250.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>x+1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.0/24</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>10.250.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>x+2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.0/24</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>10.250.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>x+7</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.0/27</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>10.250.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>x+1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.250</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>10.250.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>x+1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.249</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>10.250.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>x+1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.248</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>10.250.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>x+2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.151</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>10.250.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>x+2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.152</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>10.250.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>x+2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>.100</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>10.250.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>x</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.250</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>10.250.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>x</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.151</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>10.250.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>x</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.152</t>
-    </r>
-  </si>
-  <si>
-    <t>DSG8</t>
-  </si>
-  <si>
-    <t>DSG9</t>
-  </si>
-  <si>
-    <t>DSG10</t>
-  </si>
-  <si>
-    <t>10.250.56.0/21</t>
-  </si>
-  <si>
-    <t>10.250.64.0/21</t>
-  </si>
-  <si>
-    <t>10.250.72.0/21</t>
-  </si>
-  <si>
-    <t>Service Accounts:</t>
-  </si>
-  <si>
-    <t>User Description</t>
-  </si>
-  <si>
-    <t>User Name</t>
-  </si>
-  <si>
-    <t>Password</t>
-  </si>
-  <si>
-    <r>
-      <t>DSG</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>x</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Data Science LDAP User</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>DSG</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>x</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> GitLab LDAP User</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>DSG</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>x</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> HackMD LDAP User</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>DSG</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>x</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Test User</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>dsg</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>X</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>dsguldap</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>dsg</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>X</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>gitlabldap</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>dsg</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>X</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>hackmdldap</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>dsg</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>X</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>testuser</t>
-    </r>
-  </si>
-  <si>
-    <t>VM/Domain Admin</t>
-  </si>
-  <si>
-    <t>GitLab root</t>
-  </si>
-  <si>
-    <t>DSG Environment</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t>RADIUS Secret (Global NPS Server)</t>
-  </si>
-  <si>
-    <t>Services:</t>
-  </si>
-  <si>
-    <t>Management Environment</t>
-  </si>
-  <si>
-    <t>Domain Service Accounts:</t>
-  </si>
-  <si>
-    <t>n/a</t>
-  </si>
-  <si>
-    <t>VPN P2S SSL Certificate</t>
-  </si>
-  <si>
-    <t>root</t>
-  </si>
-  <si>
-    <t>Storage Account</t>
-  </si>
-  <si>
-    <t>Data Study Group Environment Configuration - Network</t>
-  </si>
-  <si>
-    <t>Data Study Group Environment Configuration - Service/User Accounts</t>
-  </si>
-  <si>
-    <t>Blob</t>
-  </si>
-  <si>
-    <t>URL</t>
-  </si>
-  <si>
-    <t>SAS Token</t>
-  </si>
-  <si>
-    <t>File Share</t>
-  </si>
-  <si>
-    <t>PowerShell Connection String</t>
-  </si>
-  <si>
-    <t>Data Study Group Environment Configuration - Azure</t>
-  </si>
-  <si>
-    <t>Resource Group</t>
-  </si>
-  <si>
-    <t>Virtual Network</t>
-  </si>
-  <si>
-    <t>File Share Name</t>
-  </si>
-  <si>
-    <t>RG_DSG_DC</t>
-  </si>
-  <si>
-    <t>RG_DSG_DATASERVER</t>
-  </si>
-  <si>
-    <t>RG_DSG_RDS</t>
-  </si>
-  <si>
-    <t>RG_DSG_LINUX</t>
-  </si>
-  <si>
-    <t>Data Study Group Environment Configuration - Management Environment</t>
-  </si>
-  <si>
-    <t>Domain Name</t>
-  </si>
-  <si>
-    <t>Domain Controller Name</t>
-  </si>
-  <si>
-    <t>Domain Controller IP Address</t>
-  </si>
-  <si>
-    <t>Network Policy Server Name</t>
-  </si>
-  <si>
-    <t>Network Policy Server IP Address</t>
-  </si>
-  <si>
-    <t>Domain Admin Account</t>
-  </si>
-  <si>
-    <t>FQDN of Management Domain</t>
-  </si>
-  <si>
-    <t>OU Path to HackMD LDAP User</t>
-  </si>
-  <si>
-    <t>OU Path to GitLab LDAP User</t>
-  </si>
-  <si>
-    <t>Path to Safe Haven Reseach Users OU</t>
-  </si>
-  <si>
-    <r>
-      <t>10.250.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>x+1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.0/24</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>10.250.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>x+2</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.0/24</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>10.250.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>x+7</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.0/27</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>10.250.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>x+1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.250</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>10.250.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>x+1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.249</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>10.250.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>x+1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.248</t>
     </r>
   </si>
 </sst>
@@ -1444,7 +1444,7 @@
   <dimension ref="B2:L30"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+      <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1463,7 +1463,7 @@
   <sheetData>
     <row r="2" spans="2:12" ht="19" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2"/>
@@ -1475,7 +1475,7 @@
     </row>
     <row r="4" spans="2:12" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="3" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C4" s="3"/>
     </row>
@@ -1495,7 +1495,7 @@
         <v>13</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>1</v>
@@ -1536,13 +1536,13 @@
         <v>51</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="I7" s="6" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="K7" s="6" t="s">
         <v>37</v>
@@ -1594,7 +1594,7 @@
         <v>8</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="E11" s="5" t="s">
         <v>9</v>
@@ -1626,10 +1626,10 @@
         <v>14</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F12" s="6" t="s">
         <v>2</v>
@@ -1645,18 +1645,18 @@
         <v>15</v>
       </c>
       <c r="K12" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="L12" s="6" t="s">
         <v>57</v>
-      </c>
-      <c r="L12" s="6" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="13" spans="2:12" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K13" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="L13" s="6" t="s">
         <v>58</v>
-      </c>
-      <c r="L13" s="6" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="14" spans="2:12" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1664,10 +1664,10 @@
         <v>17</v>
       </c>
       <c r="K14" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="L14" s="6" t="s">
         <v>59</v>
-      </c>
-      <c r="L14" s="6" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="15" spans="2:12" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1679,7 +1679,7 @@
         <v>8</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="E16" s="5" t="s">
         <v>9</v>
@@ -1705,10 +1705,10 @@
         <v>14</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>53</v>
+        <v>118</v>
       </c>
       <c r="F17" s="6" t="s">
         <v>4</v>
@@ -1743,7 +1743,7 @@
         <v>8</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="F21" s="5" t="s">
         <v>9</v>
@@ -1772,10 +1772,10 @@
         <v>20</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="F22" s="6" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="G22" s="6" t="s">
         <v>3</v>
@@ -1807,7 +1807,7 @@
         <v>RG_DSG_RDS</v>
       </c>
       <c r="F23" s="6" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="G23" s="6" t="s">
         <v>3</v>
@@ -1839,7 +1839,7 @@
         <v>RG_DSG_RDS</v>
       </c>
       <c r="F24" s="6" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="G24" s="6" t="s">
         <v>3</v>
@@ -1874,7 +1874,7 @@
         <v>8</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="F28" s="5" t="s">
         <v>9</v>
@@ -1903,10 +1903,10 @@
         <v>14</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="F29" s="6" t="s">
-        <v>55</v>
+        <v>116</v>
       </c>
       <c r="G29" s="6" t="s">
         <v>4</v>
@@ -1938,7 +1938,7 @@
         <v>RG_DSG_LINUX</v>
       </c>
       <c r="F30" s="6" t="s">
-        <v>56</v>
+        <v>117</v>
       </c>
       <c r="G30" s="6" t="s">
         <v>4</v>
@@ -1966,7 +1966,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D20F819-AE53-4EEF-8529-938B13ED2786}">
   <dimension ref="B2:E30"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A19" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A10" workbookViewId="0">
       <selection activeCell="D30" sqref="D30:E30"/>
     </sheetView>
   </sheetViews>
@@ -1980,7 +1980,7 @@
   <sheetData>
     <row r="2" spans="2:4" ht="19" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="3" spans="2:4" ht="19" x14ac:dyDescent="0.25">
@@ -1988,90 +1988,90 @@
     </row>
     <row r="4" spans="2:4" ht="19" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B6" s="8" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B8" s="10" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B9" s="9" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D9" s="9"/>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B10" s="9" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D10" s="9"/>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B11" s="9" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D11" s="9"/>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B12" s="9" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D12" s="9"/>
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B14" s="8" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B16" s="10" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D16" s="10" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B17" s="9" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D17" s="9"/>
     </row>
     <row r="18" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="19" spans="2:5" ht="19" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="20" spans="2:5" ht="19" x14ac:dyDescent="0.25">
@@ -2079,23 +2079,23 @@
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B21" s="8" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B23" s="10" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D23" s="10" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B24" s="9" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C24" s="9" t="s">
         <v>15</v>
@@ -2104,36 +2104,36 @@
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B25" s="13" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D25" s="9"/>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B27" s="8" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B29" s="10" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C29" s="10" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D29" s="24" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="E29" s="25"/>
     </row>
     <row r="30" spans="2:5" ht="276" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B30" s="11" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C30" s="11" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D30" s="22"/>
       <c r="E30" s="23"/>
@@ -2165,37 +2165,37 @@
     <row r="1" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="3" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="4" spans="2:3" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="5" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C4" s="11"/>
     </row>
     <row r="5" spans="2:3" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="5" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C5" s="11"/>
     </row>
     <row r="6" spans="2:3" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="5" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C6" s="11"/>
     </row>
     <row r="7" spans="2:3" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="5" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C7" s="11"/>
     </row>
     <row r="8" spans="2:3" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="20" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C8" s="21"/>
     </row>
@@ -2205,32 +2205,32 @@
     </row>
     <row r="10" spans="2:3" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="5" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C10" s="11"/>
     </row>
     <row r="11" spans="2:3" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="5" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C11" s="11"/>
     </row>
     <row r="12" spans="2:3" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="13" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B13" s="5" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="C13" s="9"/>
     </row>
     <row r="14" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B14" s="5" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C14" s="9"/>
     </row>
     <row r="15" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B15" s="5" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C15" s="9"/>
     </row>
@@ -2255,7 +2255,7 @@
   <sheetData>
     <row r="2" spans="2:5" ht="19" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="3" spans="2:5" ht="19" x14ac:dyDescent="0.25">
@@ -2263,20 +2263,20 @@
     </row>
     <row r="4" spans="2:5" ht="19" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B6" s="14" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B8" s="15" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C8" s="15" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="9" spans="2:5" ht="70.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2285,7 +2285,7 @@
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B11" s="14" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.2">
@@ -2295,10 +2295,10 @@
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B13" s="17" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C13" s="17" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="D13" s="16"/>
       <c r="E13" s="16"/>

</xml_diff>